<commit_message>
Adding moves up to L
</commit_message>
<xml_diff>
--- a/Gen8/data/database.xlsx
+++ b/Gen8/data/database.xlsx
@@ -356,7 +356,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
@@ -771,6 +771,59 @@
         </is>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Accelgor</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Adamant Orb</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Sticky Hold</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>199 HP / 96 Atk / 136 Def / 79 SpA</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Serious</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Acid Spray</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>Giga Drain</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>Guard Split</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>Feint</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>